<commit_message>
Fix bug relating to DNF being treated as PB
</commit_message>
<xml_diff>
--- a/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
+++ b/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF31F2EE-8CEE-41F2-8A03-128B250D2CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB3ADFA-EDEF-4C7D-8A13-6FC8CBD5FED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="200">
   <si>
     <t>OH</t>
   </si>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:L1049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2159,9 +2159,7 @@
       <c r="D31" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>190</v>
-      </c>
+      <c r="E31" s="12"/>
       <c r="F31" s="31">
         <v>20.54</v>
       </c>

</xml_diff>

<commit_message>
Use DNS when competitors choses not to start the solve
</commit_message>
<xml_diff>
--- a/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
+++ b/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA227D7-D9C0-4005-B728-88D5D094B3E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F37AF5-DE38-4EB2-9427-BDFC7CAD078E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="195">
   <si>
     <t>OH</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>2:39.00</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>https://www.facebook.com/events/2558750947697073/permalink/2564295957142572/</t>
@@ -1149,7 +1146,7 @@
   </sheetPr>
   <dimension ref="A1:L1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1248,7 +1245,7 @@
         <v>12.74</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F4" s="21">
         <v>14.5</v>
@@ -1283,7 +1280,7 @@
         <v>14.46</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F5" s="21">
         <v>13.82</v>
@@ -1351,7 +1348,7 @@
         <v>14.97</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="25">
         <v>13.2</v>
@@ -1386,7 +1383,7 @@
         <v>15.23</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" s="21">
         <v>14.64</v>
@@ -1421,7 +1418,7 @@
         <v>16.63</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F9" s="21">
         <v>18.3</v>
@@ -1456,7 +1453,7 @@
         <v>17.7</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F10" s="21">
         <v>14.08</v>
@@ -1575,7 +1572,7 @@
         <v>22.04</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12.75">
@@ -1592,7 +1589,7 @@
         <v>21.21</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F14" s="21">
         <v>18.43</v>
@@ -1610,7 +1607,7 @@
         <v>21.62</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75">
@@ -1627,7 +1624,7 @@
         <v>21.98</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F15" s="21">
         <v>24.1</v>
@@ -1645,7 +1642,7 @@
         <v>29.96</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75">
@@ -1662,7 +1659,7 @@
         <v>22.85</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F16" s="21">
         <v>19.38</v>
@@ -1680,7 +1677,7 @@
         <v>46.02</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="60" customFormat="1" ht="12.75">
@@ -1697,7 +1694,7 @@
         <v>25.65</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="21">
         <v>21.03</v>
@@ -1715,7 +1712,7 @@
         <v>29.2</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="12.75">
@@ -1748,7 +1745,7 @@
         <v>27.36</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75">
@@ -1756,7 +1753,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>31</v>
@@ -1783,7 +1780,7 @@
         <v>28.22</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="12.75">
@@ -1791,7 +1788,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>20</v>
@@ -1816,7 +1813,7 @@
         <v>37.68</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="12.75">
@@ -1824,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>65</v>
@@ -1849,7 +1846,7 @@
         <v>28.01</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="12.75">
@@ -1882,7 +1879,7 @@
         <v>30.93</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="12.75">
@@ -1890,7 +1887,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>20</v>
@@ -1899,7 +1896,7 @@
         <v>28.66</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F23" s="21">
         <v>29.45</v>
@@ -1917,7 +1914,7 @@
         <v>27.97</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="12.75">
@@ -1925,7 +1922,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>65</v>
@@ -1934,7 +1931,7 @@
         <v>30.91</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F24" s="21">
         <v>32.950000000000003</v>
@@ -1952,7 +1949,7 @@
         <v>32.19</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="12.75">
@@ -1985,7 +1982,7 @@
         <v>30.67</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="12.75">
@@ -1993,7 +1990,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>31</v>
@@ -2017,7 +2014,7 @@
         <v>34.72</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75">
@@ -2025,7 +2022,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>65</v>
@@ -2034,7 +2031,7 @@
         <v>34.840000000000003</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F27" s="19">
         <v>30.53</v>
@@ -2052,7 +2049,7 @@
         <v>31.2</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="12.75">
@@ -2060,7 +2057,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>31</v>
@@ -2087,7 +2084,7 @@
         <v>31.64</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="12.75">
@@ -2095,7 +2092,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="23" t="s">
         <v>65</v>
@@ -2122,7 +2119,7 @@
         <v>39.840000000000003</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75">
@@ -2130,7 +2127,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>31</v>
@@ -2155,7 +2152,7 @@
         <v>40.14</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="12.75">
@@ -2188,7 +2185,7 @@
         <v>92</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="12.75">
@@ -2196,7 +2193,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>31</v>
@@ -2221,7 +2218,7 @@
         <v>41</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12.75">
@@ -10556,7 +10553,7 @@
   <dimension ref="A1:L1034"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10654,7 +10651,7 @@
         <v>25.73</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="19">
         <v>22.13</v>
@@ -10689,7 +10686,7 @@
         <v>27.32</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="19">
         <v>23.86</v>
@@ -10759,7 +10756,7 @@
         <v>35.44</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="19">
         <v>46.11</v>
@@ -10794,7 +10791,7 @@
         <v>37.28</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" s="19">
         <v>37.57</v>
@@ -11065,14 +11062,14 @@
       <c r="H16" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="I16" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>142</v>
+      <c r="I16" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="12.75">
@@ -17549,7 +17546,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>22</v>
@@ -17584,7 +17581,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>34</v>
@@ -17619,7 +17616,7 @@
         <v>44</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>46</v>
@@ -17654,7 +17651,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>56</v>
@@ -24254,7 +24251,7 @@
   </sheetPr>
   <dimension ref="A1:L1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -24273,7 +24270,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="61" t="s">
         <v>1</v>
@@ -24282,7 +24279,7 @@
       <c r="D1" s="62"/>
       <c r="E1" s="62"/>
       <c r="F1" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -24312,13 +24309,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>177</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>178</v>
       </c>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
@@ -24341,10 +24338,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
@@ -24356,7 +24353,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="56" t="s">
         <v>31</v>
@@ -24365,10 +24362,10 @@
         <v>27</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
@@ -24389,10 +24386,10 @@
         <v>29</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
@@ -24404,7 +24401,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>20</v>
@@ -24414,7 +24411,7 @@
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
@@ -24426,7 +24423,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>20</v>
@@ -24435,10 +24432,10 @@
         <v>41</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
@@ -24450,7 +24447,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C9" s="56" t="s">
         <v>20</v>
@@ -24460,7 +24457,7 @@
       </c>
       <c r="E9" s="57"/>
       <c r="F9" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
@@ -24472,7 +24469,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>65</v>
@@ -24481,10 +24478,10 @@
         <v>55</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>

</xml_diff>

<commit_message>
FIx up some avergages - OH and 5x5x5
</commit_message>
<xml_diff>
--- a/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
+++ b/data/2020-02-24/Senior Cubers Worldwide - Weekly Competition - 2020-02-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F37AF5-DE38-4EB2-9427-BDFC7CAD078E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F33EA93-148C-494D-9795-279253622941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
   <si>
     <t>OH</t>
   </si>
@@ -610,6 +610,9 @@
   <si>
     <t>https://www.facebook.com/events/2558750947697073/permalink/2564590157113152/</t>
   </si>
+  <si>
+    <t>2:27.00</t>
+  </si>
 </sst>
 </file>
 
@@ -777,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -923,6 +926,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -10553,7 +10559,7 @@
   <dimension ref="A1:L1034"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11049,8 +11055,8 @@
       <c r="C16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>139</v>
+      <c r="D16" s="61" t="s">
+        <v>195</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="27" t="s">
@@ -17447,8 +17453,8 @@
   </sheetPr>
   <dimension ref="A1:L1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -17880,7 +17886,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="27" t="s">
@@ -24251,7 +24257,7 @@
   </sheetPr>
   <dimension ref="A1:L1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -24272,12 +24278,12 @@
       <c r="A1" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="6" t="s">
         <v>174</v>
       </c>

</xml_diff>